<commit_message>
PPP instructions for students
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\Documents\GitHub\Mandy-PhD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FD3B93-9D39-49E4-8FEC-AB3BF3E40CD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCD4FD9-AA2F-4000-A9AD-AAD7F1AD239C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Erledigt</t>
   </si>
@@ -186,7 +186,13 @@
     <t>eigene Testung organisieren bei Schulbesuch (Sportunterricht filmen etc) --&gt; in Arbeit</t>
   </si>
   <si>
-    <t>EV-Erklärung + Probandeninfo + Datenschutz</t>
+    <t>Zeit bei Prozedur nochmals überarbeiten! --&gt; Fragebogen nach JEDER Unit!</t>
+  </si>
+  <si>
+    <t>Farbe für Marker eintragen</t>
+  </si>
+  <si>
+    <t>EV-Erklärung + Probandeninfo + Datenschutz (Montag mit Franzi+Carola; Mittwoch mit Gregor)</t>
   </si>
 </sst>
 </file>
@@ -277,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -286,7 +292,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -294,9 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -611,11 +614,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -684,10 +687,10 @@
       <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="12"/>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
@@ -698,13 +701,13 @@
       <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="12"/>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
@@ -715,10 +718,10 @@
       <c r="E6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -738,10 +741,10 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -751,10 +754,10 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>31</v>
       </c>
     </row>
@@ -764,7 +767,7 @@
       <c r="D10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>39</v>
       </c>
     </row>
@@ -785,187 +788,233 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="15"/>
+      <c r="E15" s="14"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="15"/>
-    </row>
-    <row r="17" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="D17" s="16" t="s">
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="D17" s="15" t="s">
         <v>48</v>
       </c>
+      <c r="E17" s="14"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="9">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="D18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="D19" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="8">
         <v>1</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="D19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="B20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="8">
+        <v>2</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="D21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="8">
+        <v>3</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="D22" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="8">
+        <v>4</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="D23" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="8">
+        <v>5</v>
+      </c>
+      <c r="B24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="8">
+        <v>6</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="D25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="9">
-        <v>2</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="D20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="4" t="s">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="8">
+        <v>7</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="E26" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="9">
-        <v>3</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="D21" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="9">
-        <v>4</v>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="D22" s="18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="9">
-        <v>5</v>
-      </c>
-      <c r="B23" s="9"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="9">
-        <v>6</v>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="D24" s="4" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="8">
+        <v>8</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="D27" s="14"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="8">
+        <v>9</v>
+      </c>
+      <c r="B28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="8">
+        <v>10</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="D29" s="14"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="8">
+        <v>11</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="D30" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="9">
-        <v>7</v>
-      </c>
-      <c r="B25" s="9"/>
-    </row>
-    <row r="26" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="8">
+        <v>12</v>
+      </c>
+      <c r="B31" s="8"/>
+    </row>
+    <row r="32" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="9">
+        <v>13</v>
+      </c>
+      <c r="B32" s="9"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="11"/>
-      <c r="B40" s="11"/>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update infoschreiben + marker ppp
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\Documents\GitHub\Mandy-PhD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D11881B-4AC5-4B85-B0C5-7099F44FD6FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B281FC57-E37D-4B86-8A89-1FAA6A360491}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="to dos" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Erledigt</t>
   </si>
@@ -141,9 +141,6 @@
     <t>Lebenslauf</t>
   </si>
   <si>
-    <t xml:space="preserve">Abschlusszeugnis Hochschulzugang+StEx </t>
-  </si>
-  <si>
     <t>Anschreiben</t>
   </si>
   <si>
@@ -180,9 +177,6 @@
     <t>Counterbalancing</t>
   </si>
   <si>
-    <t>Technik aufbauen + im Raum testen --&gt; Schlüssel?</t>
-  </si>
-  <si>
     <t>eigene Testung organisieren bei Schulbesuch (Sportunterricht filmen etc) --&gt; in Arbeit</t>
   </si>
   <si>
@@ -196,6 +190,21 @@
   </si>
   <si>
     <t>MARKER: 3 Videos je 10 sec; marker allein, marker front back, fläche mit 4 markern</t>
+  </si>
+  <si>
+    <t>Fragebogen fertigstellen + ausdrucken</t>
+  </si>
+  <si>
+    <t>Infomail mit Instruktionen an Carola, Gereon, Franzi, Gregor</t>
+  </si>
+  <si>
+    <t>Folie für Fragen in PPP einbauen</t>
+  </si>
+  <si>
+    <t>Technik aufbauen + im Raum testen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abschlusszeugnis StEx </t>
   </si>
 </sst>
 </file>
@@ -265,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -282,18 +291,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -305,6 +321,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -619,11 +638,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -692,10 +711,10 @@
       <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
@@ -706,13 +725,13 @@
       <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="11"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
@@ -723,10 +742,10 @@
       <c r="E6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -746,10 +765,10 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="11" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -759,10 +778,10 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>31</v>
       </c>
     </row>
@@ -772,8 +791,8 @@
       <c r="D10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>39</v>
+      <c r="E10" s="10" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -793,244 +812,261 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
-      <c r="D13" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="14" t="s">
+      <c r="D13" s="12" t="s">
         <v>40</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
-      <c r="D14" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="14"/>
+      <c r="D14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="12"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
-      <c r="D15" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="14"/>
+      <c r="D15" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
-      <c r="D16" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="14"/>
+      <c r="D16" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
-      <c r="D17" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="14"/>
+      <c r="D17" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="D18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="D19" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
-      <c r="D19" s="14" t="s">
+    </row>
+    <row r="20" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="D20" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="D21" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="D22" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="16"/>
+      <c r="B23" s="17"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="6">
+        <v>1</v>
+      </c>
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="6">
+        <v>2</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="D25" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="6">
+        <v>3</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="D26" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="6">
+        <v>4</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="D27" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="6">
+        <v>5</v>
+      </c>
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="6">
+        <v>6</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="D29" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="6">
+        <v>7</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="D30" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="6">
+        <v>8</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="D31" s="12"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="6">
+        <v>9</v>
+      </c>
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="6">
+        <v>10</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="D33" s="12"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="6">
+        <v>11</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="D34" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="D20" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="D21" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="8">
-        <v>1</v>
-      </c>
-      <c r="B22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="8">
-        <v>2</v>
-      </c>
-      <c r="B23" s="8"/>
-      <c r="D23" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="8">
-        <v>3</v>
-      </c>
-      <c r="B24" s="8"/>
-      <c r="D24" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="8">
-        <v>4</v>
-      </c>
-      <c r="B25" s="8"/>
-      <c r="F25" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="8">
-        <v>5</v>
-      </c>
-      <c r="B26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="8">
-        <v>6</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="E27" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="8">
-        <v>7</v>
-      </c>
-      <c r="B28" s="8"/>
-      <c r="D28" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="8">
-        <v>8</v>
-      </c>
-      <c r="B29" s="8"/>
-      <c r="D29" s="14"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="8">
-        <v>9</v>
-      </c>
-      <c r="B30" s="8"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="8">
-        <v>10</v>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="D31" s="14"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="8">
-        <v>11</v>
-      </c>
-      <c r="B32" s="8"/>
-      <c r="D32" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="8">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="6">
         <v>12</v>
       </c>
-      <c r="B33" s="8"/>
-    </row>
-    <row r="34" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="9">
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="7">
         <v>13</v>
       </c>
-      <c r="B34" s="9"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10" t="s">
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G35" s="4" t="s">
+      <c r="C37" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="10"/>
-      <c r="B36" s="10"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-    </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="10"/>
-      <c r="B47" s="10"/>
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update to do + mocklist
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\Documents\GitHub\Mandy-PhD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\empschulml\Documents\GitHub\Mandy-PhD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E263E816-E5A6-4D16-BB35-66CFF097471E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD0CB3B-9E32-45A6-9D07-ACF02EFA7090}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="to dos" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Erledigt</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>DICKES CHECK :-D</t>
+  </si>
+  <si>
+    <t>Mail für nä Wo Mi schreiben</t>
+  </si>
+  <si>
+    <t>ET Videos kodieren</t>
   </si>
 </sst>
 </file>
@@ -334,8 +340,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -650,26 +656,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="28" style="4" customWidth="1"/>
-    <col min="4" max="4" width="37.81640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="40.81640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="27.81640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="25.54296875" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="10.81640625" style="4"/>
+    <col min="4" max="4" width="37.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="10.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -689,13 +695,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
@@ -711,7 +717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
@@ -728,7 +734,7 @@
       </c>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4" t="s">
@@ -745,7 +751,7 @@
       </c>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
@@ -761,7 +767,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
@@ -774,7 +780,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="10" t="s">
@@ -790,7 +796,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="D9" s="10" t="s">
@@ -800,7 +806,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="D10" s="4" t="s">
@@ -810,7 +816,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="D11" s="4" t="s">
@@ -820,7 +826,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="D12" s="12" t="s">
@@ -830,7 +836,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="D13" s="12" t="s">
@@ -840,7 +846,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="D14" s="10" t="s">
@@ -850,17 +856,17 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="D15" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="20" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="D16" s="13" t="s">
@@ -868,7 +874,7 @@
       </c>
       <c r="E16" s="12"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="D17" s="4" t="s">
@@ -878,212 +884,234 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="D18" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="D19" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="D20" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="D21" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="D22" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="D23" s="20" t="s">
+    <row r="23" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="D23" s="21" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6">
+    <row r="24" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="15"/>
+      <c r="D24" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="15"/>
+      <c r="D25" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="15"/>
+      <c r="D26" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="16"/>
+      <c r="B27" s="17"/>
+      <c r="D27" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
         <v>1</v>
       </c>
-      <c r="B24" s="6"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="6">
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
         <v>2</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="D25" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="4" t="s">
+      <c r="B29" s="6"/>
+      <c r="D29" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G29" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="6">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
         <v>3</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="D26" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="6">
+      <c r="B30" s="6"/>
+      <c r="D30" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
         <v>4</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="D27" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="6">
+      <c r="B31" s="6"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
         <v>5</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="D28" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="6">
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
         <v>6</v>
       </c>
-      <c r="B29" s="6"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="6">
+      <c r="B33" s="6"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
         <v>7</v>
       </c>
-      <c r="B30" s="6"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="6">
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
         <v>8</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="D31" s="12"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="6">
+      <c r="B35" s="6"/>
+      <c r="D35" s="12"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
         <v>9</v>
       </c>
-      <c r="B32" s="6"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="6">
+      <c r="B36" s="6"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
         <v>10</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="D33" s="12"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="6">
+      <c r="B37" s="6"/>
+      <c r="D37" s="12"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
         <v>11</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="D34" s="12" t="s">
+      <c r="B38" s="6"/>
+      <c r="D38" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="6">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
         <v>12</v>
       </c>
-      <c r="B35" s="6"/>
-    </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="7">
+      <c r="B39" s="6"/>
+    </row>
+    <row r="40" spans="1:7" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7">
         <v>13</v>
       </c>
-      <c r="B36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8" t="s">
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G41" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
+      <c r="B53" s="8"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update fragebogen items + todos
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\Documents\GitHub\Mandy-PhD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52BF9D1-0E7D-478D-A4C8-F8DB307343B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D222DC-42A0-40E0-90AB-25169C9DF0D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Erledigt</t>
   </si>
@@ -210,35 +210,56 @@
     <t>Fragebogen fertigstellen + ausdrucken</t>
   </si>
   <si>
-    <t>DICKES CHECK :-D</t>
-  </si>
-  <si>
     <t>Ethikantrag überarbeiten --&gt; siehe Server</t>
   </si>
   <si>
-    <t>Videos mit BORIS kodieren</t>
-  </si>
-  <si>
     <t>Fragebogen einpflegen --&gt; siehe Eva, Server</t>
   </si>
   <si>
     <t xml:space="preserve">ET Videos exportieren mit metrics --&gt; GRI berechnen </t>
   </si>
   <si>
-    <t xml:space="preserve">mockliste ins paper hämmern </t>
-  </si>
-  <si>
-    <t>eigene Testung organisieren bei Schulbesuch (Sportunterricht filmen etc) --&gt; Montag, 10.08. erster Test in Turnhalle</t>
-  </si>
-  <si>
     <t>Videos schneiden --&gt; DaVinci</t>
+  </si>
+  <si>
+    <t>Coffee Club PPP vorbereiten für Mittwoch, 19.08.2020</t>
+  </si>
+  <si>
+    <t>eigene Testung organisieren bei Schulbesuch (Sportunterricht filmen etc) --&gt; Kontaktaufnahme mit Lehrer:innen ist erfolgt</t>
+  </si>
+  <si>
+    <t>Videos mit BORIS kodieren: Codingschema erstellen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mockliste ins Paper hämmern </t>
+  </si>
+  <si>
+    <t>DICKES CHECK</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nächster Promotionsausschuss: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>16.09.2020</t>
+    </r>
+  </si>
+  <si>
+    <t>Konferenz in Antwerpen --&gt; Infos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,8 +297,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,12 +360,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -341,11 +405,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -369,10 +452,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Berechnung" xfId="4" builtinId="22"/>
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -689,7 +780,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -697,9 +788,9 @@
     <col min="1" max="1" width="4" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.81640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="28" style="4" customWidth="1"/>
-    <col min="4" max="4" width="99.6328125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="102.1796875" style="4" customWidth="1"/>
     <col min="5" max="5" width="18.1796875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="27.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="45.26953125" style="4" customWidth="1"/>
     <col min="7" max="7" width="25.54296875" style="4" customWidth="1"/>
     <col min="8" max="16384" width="10.81640625" style="4"/>
   </cols>
@@ -845,7 +936,7 @@
         <v>38</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -894,6 +985,9 @@
       <c r="D15" s="13" t="s">
         <v>45</v>
       </c>
+      <c r="E15" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
@@ -909,9 +1003,6 @@
       <c r="D17" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
@@ -919,6 +1010,9 @@
       <c r="D18" s="12" t="s">
         <v>48</v>
       </c>
+      <c r="E18" s="20" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="19" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14"/>
@@ -933,6 +1027,9 @@
       <c r="D20" s="12" t="s">
         <v>49</v>
       </c>
+      <c r="E20" s="12" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="21" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14"/>
@@ -961,9 +1058,6 @@
       <c r="D24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="20" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="25" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14"/>
@@ -997,11 +1091,11 @@
         <v>2</v>
       </c>
       <c r="B29" s="6"/>
-      <c r="C29" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="23" t="s">
-        <v>63</v>
+      <c r="C29" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>64</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>29</v>
@@ -1015,14 +1109,17 @@
         <v>3</v>
       </c>
       <c r="B30" s="6"/>
+      <c r="D30" s="25" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
         <v>4</v>
       </c>
       <c r="B31" s="6"/>
-      <c r="D31" s="23" t="s">
-        <v>64</v>
+      <c r="F31" s="23" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -1030,14 +1127,20 @@
         <v>5</v>
       </c>
       <c r="B32" s="6"/>
+      <c r="D32" s="25" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>6</v>
       </c>
       <c r="B33" s="6"/>
-      <c r="D33" s="23" t="s">
-        <v>65</v>
+      <c r="D33" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -1051,9 +1154,6 @@
         <v>8</v>
       </c>
       <c r="B35" s="6"/>
-      <c r="D35" s="24" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="6">
@@ -1073,8 +1173,8 @@
         <v>11</v>
       </c>
       <c r="B38" s="6"/>
-      <c r="D38" s="12" t="s">
-        <v>67</v>
+      <c r="D38" s="28" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>